<commit_message>
update os and network
</commit_message>
<xml_diff>
--- a/01 秋招资料/招聘信息汇总.xlsx
+++ b/01 秋招资料/招聘信息汇总.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/iiixv/Documents/Notebook/01 秋招资料/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B4897F7-E9C6-714B-812C-6EB93BB64A73}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C10D245-772B-0849-BA13-DC5C378DD5D4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{F54258CB-92F9-234B-A0D3-16063D77C905}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="174">
   <si>
     <t>企业名称</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -518,10 +518,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>笔试</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>筛选</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -620,6 +616,71 @@
   <si>
     <t>校招-后端开发工程师-整车研发（第二志愿）</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>深信服</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://app.mokahr.com/campus_apply/sangfor/27944#/?anchorName=default_banner&amp;sourceToken=</t>
+  </si>
+  <si>
+    <t>筛选(提前批)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://app.mokahr.com/campus_apply/sangfor/27944#/candidateHome/applications</t>
+  </si>
+  <si>
+    <t>Python开发工程师（提前批 成都）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://campus.mihoyo.com/#/campus</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>筛选中</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://campus.mihoyo.com/#/campus/applyRecord</t>
+  </si>
+  <si>
+    <t>Java后端开发工程师</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>滴滴</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://campus.didiglobal.com/campus_apply/didiglobal/6223#/?anchorName=default_banner&amp;sourceToken=</t>
+  </si>
+  <si>
+    <t>https://campus.didiglobal.com/campus_apply/didiglobal/6223#/candidateHome/applications</t>
+  </si>
+  <si>
+    <t>笔试（结束）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>筛选（已处理）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://careers.cvte.com/zone/resume/applications</t>
+  </si>
+  <si>
+    <t>笔试(08-31)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>视源股份(提前批)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Web后台开发工程师 </t>
   </si>
 </sst>
 </file>
@@ -674,7 +735,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -684,6 +745,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -720,7 +793,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -749,6 +822,18 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1068,8 +1153,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5272D451-109C-3F4D-8230-0B9995B3B1B8}">
   <dimension ref="A1:I45"/>
   <sheetViews>
-    <sheetView topLeftCell="A33" zoomScale="110" workbookViewId="0">
-      <selection activeCell="D46" sqref="D46"/>
+    <sheetView zoomScale="110" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1808,7 +1893,7 @@
     </row>
     <row r="45" spans="1:9">
       <c r="A45" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C45" s="8">
         <v>44781</v>
@@ -1841,8 +1926,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80C510C1-FE06-2A40-90B2-49BDE09299BE}">
   <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1901,7 +1986,7 @@
         <v>44788</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>109</v>
@@ -1931,7 +2016,7 @@
         <v>44788</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>113</v>
@@ -1961,7 +2046,7 @@
         <v>44788</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1" t="s">
@@ -1985,7 +2070,7 @@
         <v>44788</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E5" s="5" t="s">
         <v>126</v>
@@ -2002,29 +2087,29 @@
       <c r="I5" s="9"/>
       <c r="J5" s="1"/>
     </row>
-    <row r="6" spans="1:10" ht="46">
-      <c r="A6" s="1" t="s">
+    <row r="6" spans="1:10" s="12" customFormat="1" ht="46">
+      <c r="A6" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="10" t="s">
         <v>116</v>
       </c>
-      <c r="C6" s="9">
+      <c r="C6" s="11">
         <v>44754</v>
       </c>
-      <c r="D6" s="9" t="s">
-        <v>129</v>
-      </c>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1" t="s">
+      <c r="D6" s="11" t="s">
+        <v>168</v>
+      </c>
+      <c r="E6" s="10"/>
+      <c r="F6" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="G6" s="1"/>
-      <c r="H6" s="9"/>
-      <c r="I6" s="9" t="s">
+      <c r="G6" s="10"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="J6" s="1"/>
+      <c r="J6" s="10"/>
     </row>
     <row r="7" spans="1:10" s="3" customFormat="1" ht="46">
       <c r="A7" s="1" t="s">
@@ -2037,7 +2122,7 @@
         <v>44788</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>130</v>
+        <v>169</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>121</v>
@@ -2050,7 +2135,7 @@
       <c r="I7" s="9"/>
       <c r="J7" s="1"/>
     </row>
-    <row r="8" spans="1:10" ht="92">
+    <row r="8" spans="1:10" ht="51">
       <c r="A8" s="1">
         <v>360</v>
       </c>
@@ -2061,9 +2146,9 @@
         <v>44788</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>130</v>
-      </c>
-      <c r="E8" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="E8" s="5" t="s">
         <v>127</v>
       </c>
       <c r="F8" s="1" t="s">
@@ -2076,27 +2161,27 @@
       <c r="I8" s="9"/>
       <c r="J8" s="1"/>
     </row>
-    <row r="9" spans="1:10" ht="69">
+    <row r="9" spans="1:10" ht="34">
       <c r="A9" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C9" s="9">
         <v>44791</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>130</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>133</v>
+        <v>129</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>132</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>119</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H9" s="9"/>
       <c r="I9" s="9"/>
@@ -2104,22 +2189,22 @@
     </row>
     <row r="10" spans="1:10" ht="23">
       <c r="A10" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C10" s="9">
         <v>44791</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G10" s="1"/>
       <c r="H10" s="9"/>
@@ -2128,22 +2213,22 @@
     </row>
     <row r="11" spans="1:10" ht="46">
       <c r="A11" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C11" s="9">
         <v>44791</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G11" s="1"/>
       <c r="H11" s="9"/>
@@ -2152,22 +2237,22 @@
     </row>
     <row r="12" spans="1:10" ht="46">
       <c r="A12" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C12" s="9">
         <v>44792</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="G12" s="1"/>
       <c r="H12" s="9"/>
@@ -2185,13 +2270,13 @@
         <v>44792</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E13" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="F13" s="1" t="s">
         <v>149</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>150</v>
       </c>
       <c r="G13" s="1"/>
       <c r="H13" s="9"/>
@@ -2200,22 +2285,22 @@
     </row>
     <row r="14" spans="1:10" ht="46">
       <c r="A14" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>152</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>153</v>
       </c>
       <c r="C14" s="9">
         <v>44792</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="G14" s="1"/>
       <c r="H14" s="9"/>
@@ -2233,62 +2318,110 @@
         <v>44792</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E15" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="F15" s="1" t="s">
         <v>155</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>156</v>
       </c>
       <c r="G15" s="1"/>
       <c r="H15" s="9"/>
       <c r="I15" s="9"/>
       <c r="J15" s="1"/>
     </row>
-    <row r="16" spans="1:10" ht="22">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="9"/>
-      <c r="D16" s="9"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
+    <row r="16" spans="1:10" ht="69">
+      <c r="A16" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="C16" s="9">
+        <v>44793</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>158</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>160</v>
+      </c>
       <c r="G16" s="1"/>
       <c r="H16" s="9"/>
       <c r="I16" s="9"/>
       <c r="J16" s="1"/>
     </row>
-    <row r="17" spans="1:10" ht="22">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
-      <c r="C17" s="9"/>
-      <c r="D17" s="9"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
+    <row r="17" spans="1:10" ht="23">
+      <c r="A17" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="C17" s="9">
+        <v>44797</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>162</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>164</v>
+      </c>
       <c r="G17" s="1"/>
       <c r="H17" s="9"/>
       <c r="I17" s="9"/>
       <c r="J17" s="1"/>
     </row>
-    <row r="18" spans="1:10" ht="22">
-      <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
-      <c r="C18" s="9"/>
-      <c r="D18" s="9"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
+    <row r="18" spans="1:10" ht="69">
+      <c r="A18" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="C18" s="9">
+        <v>44797</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>158</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>112</v>
+      </c>
       <c r="G18" s="1"/>
       <c r="H18" s="9"/>
       <c r="I18" s="9"/>
       <c r="J18" s="1"/>
     </row>
-    <row r="19" spans="1:10" ht="22">
-      <c r="A19" s="1"/>
-      <c r="B19" s="1"/>
-      <c r="C19" s="9"/>
-      <c r="D19" s="9"/>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
+    <row r="19" spans="1:10" ht="46">
+      <c r="A19" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="C19" s="9">
+        <v>44797</v>
+      </c>
+      <c r="D19" s="13" t="s">
+        <v>171</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>173</v>
+      </c>
       <c r="G19" s="1"/>
       <c r="H19" s="9"/>
       <c r="I19" s="9"/>
@@ -2419,6 +2552,9 @@
     <hyperlink ref="E10" r:id="rId12" xr:uid="{CC88F09B-AA15-DD4B-9C2F-777C896A0449}"/>
     <hyperlink ref="B13" r:id="rId13" xr:uid="{9C156E97-C328-344D-B61B-154767D86E41}"/>
     <hyperlink ref="E13" r:id="rId14" xr:uid="{884DAFF2-096B-0948-9C47-9678F5D3F8AE}"/>
+    <hyperlink ref="B17" r:id="rId15" location="/campus" xr:uid="{D8F58B25-FC40-4D4D-AE09-2339F2318B69}"/>
+    <hyperlink ref="E8" r:id="rId16" xr:uid="{3FCD14E2-3D91-2445-92CD-4CE114D8A151}"/>
+    <hyperlink ref="E9" r:id="rId17" location="/candidateHome/applications" xr:uid="{3EDE88CC-9364-4947-9430-80F6E2905C15}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>